<commit_message>
Update: BCRPP Warning Rules
edits to warning rules for:

alcohol_amt - increased upper limit to 42 g/day 
parous - if parous =0, allow parity to have values of 0 or 888
screen_ever -if screen_ever=0, allow lastscreen_year to have values of 777 or 7777
</commit_message>
<xml_diff>
--- a/BCRPP_QC_R_Excel_Program/BCRPP_QC_DataDictionary_Version_1/Core QC Rules/BCRPP Warning Rules.xlsx
+++ b/BCRPP_QC_R_Excel_Program/BCRPP_QC_DataDictionary_Version_1/Core QC Rules/BCRPP Warning Rules.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FC5E05-88D5-4EAE-B9E8-BC9DD845BE04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A88CCA-E95C-4BF6-948A-EC450C4C0256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-76920" yWindow="-5820" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="353">
   <si>
     <t>Variable</t>
   </si>
@@ -518,12 +518,6 @@
     <t>alcohol_amt</t>
   </si>
   <si>
-    <t>alcohol_amt &gt; 0 &amp; alcohol_amt &lt;= 25 | alcohol_amt == 888</t>
-  </si>
-  <si>
-    <t>Verify: alcohol_amt is outside range 0-25 gms</t>
-  </si>
-  <si>
     <t xml:space="preserve">alcohol_stop </t>
   </si>
   <si>
@@ -1092,6 +1086,15 @@
   </si>
   <si>
     <t xml:space="preserve">Verify Parity: Parous=1, but parity less than 1 or more than 15 pregnancies  </t>
+  </si>
+  <si>
+    <t>alcohol_amt &gt; 0 &amp; alcohol_amt &lt; 42 | alcohol_amt == 888</t>
+  </si>
+  <si>
+    <t>Verify: alcohol_amt is outside range 0-42 gms</t>
+  </si>
+  <si>
+    <t>777, 7777</t>
   </si>
 </sst>
 </file>
@@ -1466,8 +1469,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G64" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88:G88"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="I93" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="M109" sqref="M109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -1877,7 +1883,7 @@
         <v>63</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.45">
@@ -2222,7 +2228,7 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>21</v>
@@ -2232,10 +2238,10 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>112</v>
@@ -2252,10 +2258,10 @@
       <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
       <c r="S35" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="T35" s="3" t="s">
         <v>349</v>
-      </c>
-      <c r="T35" s="3" t="s">
-        <v>351</v>
       </c>
       <c r="U35" s="3"/>
     </row>
@@ -2276,13 +2282,13 @@
         <v>98</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="S36" s="2" t="s">
         <v>80</v>
       </c>
       <c r="T36" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.45">
@@ -2296,19 +2302,19 @@
         <v>101</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>98</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="S37" s="2" t="s">
         <v>82</v>
       </c>
       <c r="T37" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.45">
@@ -2322,19 +2328,19 @@
         <v>102</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>98</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="S38" s="2" t="s">
         <v>84</v>
       </c>
       <c r="T38" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.45">
@@ -2348,19 +2354,19 @@
         <v>103</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>98</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="S39" s="2" t="s">
         <v>86</v>
       </c>
       <c r="T39" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.45">
@@ -2374,19 +2380,19 @@
         <v>104</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>98</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="S40" s="2" t="s">
         <v>88</v>
       </c>
       <c r="T40" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.45">
@@ -2400,19 +2406,19 @@
         <v>105</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>98</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="S41" s="2" t="s">
         <v>90</v>
       </c>
       <c r="T41" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.45">
@@ -2426,19 +2432,19 @@
         <v>106</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>98</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="S42" s="2" t="s">
         <v>92</v>
       </c>
       <c r="T42" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.45">
@@ -2452,19 +2458,19 @@
         <v>107</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>108</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="S43" s="2" t="s">
         <v>94</v>
       </c>
       <c r="T43" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.45">
@@ -2478,19 +2484,19 @@
         <v>109</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>98</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="S44" s="2" t="s">
         <v>96</v>
       </c>
       <c r="T44" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.45">
@@ -2510,7 +2516,7 @@
         <v>110</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>112</v>
@@ -2548,7 +2554,7 @@
         <v>110</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>112</v>
@@ -2586,7 +2592,7 @@
         <v>119</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>112</v>
@@ -2624,7 +2630,7 @@
         <v>122</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>112</v>
@@ -2662,7 +2668,7 @@
         <v>125</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>112</v>
@@ -2700,7 +2706,7 @@
         <v>128</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>112</v>
@@ -2738,7 +2744,7 @@
         <v>131</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>112</v>
@@ -2776,7 +2782,7 @@
         <v>134</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>112</v>
@@ -2814,7 +2820,7 @@
         <v>137</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I53" s="2" t="s">
         <v>112</v>
@@ -2852,7 +2858,7 @@
         <v>140</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>112</v>
@@ -2985,7 +2991,7 @@
         <v>155</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>147</v>
@@ -2997,7 +3003,7 @@
         <v>147</v>
       </c>
       <c r="T59" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.45">
@@ -3034,7 +3040,7 @@
         <v>159</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="I61" s="2" t="s">
         <v>143</v>
@@ -3046,7 +3052,7 @@
         <v>159</v>
       </c>
       <c r="T61" s="2" t="s">
-        <v>161</v>
+        <v>351</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.45">
@@ -3060,19 +3066,19 @@
         <v>148</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I62" s="2" t="s">
         <v>143</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="S62" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="T62" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.45">
@@ -3086,192 +3092,192 @@
         <v>149</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I63" s="2" t="s">
         <v>143</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="S63" s="2" t="s">
         <v>149</v>
       </c>
       <c r="T63" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A64" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G64" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I64" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="H64" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="I64" s="2" t="s">
+      <c r="J64" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="S64" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="T64" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="J64" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="S64" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="T64" s="2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A65" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J65" s="2">
         <v>1</v>
       </c>
       <c r="S65" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="T65" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="T65" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A66" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="S66" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="T66" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A67" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G67" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="S67" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="T67" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="I67" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="J67" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="S67" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="T67" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>111</v>
       </c>
       <c r="G68" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="J68" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="L68" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="M68" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="S68" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="T68" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="I68" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="J68" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="L68" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="M68" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="S68" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="T68" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A69" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>111</v>
       </c>
       <c r="G69" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="J69" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="L69" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="M69" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="H69" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="I69" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="J69" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="L69" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="M69" s="2" t="s">
-        <v>182</v>
-      </c>
       <c r="S69" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="T69" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A70" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>146</v>
@@ -3280,33 +3286,33 @@
         <v>4</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O70" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="P70" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="S70" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="T70" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A71" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>37</v>
@@ -3315,157 +3321,157 @@
         <v>1</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J71" s="2">
         <v>666</v>
       </c>
       <c r="S71" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="T71" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A72" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>111</v>
       </c>
       <c r="G72" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I72" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="H72" s="2" t="s">
+      <c r="J72" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="I72" s="2" t="s">
+      <c r="L72" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="M72" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="S72" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="T72" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="J72" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="L72" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="M72" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="S72" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="T72" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A73" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J73" s="2">
         <v>1</v>
       </c>
       <c r="S73" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="T73" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J74" s="2">
         <v>0</v>
       </c>
       <c r="S74" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="T74" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="T74" s="2" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A75" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J75" s="2">
         <v>888</v>
       </c>
       <c r="S75" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="T75" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A76" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J76" s="2">
         <v>1</v>
       </c>
       <c r="S76" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="T76" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>37</v>
@@ -3474,21 +3480,21 @@
         <v>0</v>
       </c>
       <c r="I77" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="J77" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="S77" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="T77" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="J77" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="S77" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="T77" s="2" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A78" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>37</v>
@@ -3497,16 +3503,16 @@
         <v>888</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J78" s="2">
         <v>888</v>
       </c>
       <c r="S78" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="T78" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.45">
@@ -3528,11 +3534,11 @@
       <c r="L79" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="M79" s="2">
-        <v>0</v>
+      <c r="M79" s="2" t="s">
+        <v>294</v>
       </c>
       <c r="O79" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="P79" s="2">
         <v>777</v>
@@ -3541,7 +3547,7 @@
         <v>112</v>
       </c>
       <c r="T79" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.45">
@@ -3567,7 +3573,7 @@
         <v>888</v>
       </c>
       <c r="O80" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="P80" s="2">
         <v>888</v>
@@ -3576,7 +3582,7 @@
         <v>112</v>
       </c>
       <c r="T80" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.45">
@@ -3596,19 +3602,19 @@
         <v>98</v>
       </c>
       <c r="J81" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L81" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="M81" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="S81" s="2" t="s">
         <v>112</v>
       </c>
       <c r="T81" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.45">
@@ -3622,7 +3628,7 @@
         <v>0</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="J82" s="2">
         <v>777</v>
@@ -3631,12 +3637,12 @@
         <v>112</v>
       </c>
       <c r="T82" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A83" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>37</v>
@@ -3645,21 +3651,21 @@
         <v>0</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="J83" s="2">
         <v>666</v>
       </c>
       <c r="S83" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="T83" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A84" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>34</v>
@@ -3671,15 +3677,15 @@
         <v>84</v>
       </c>
       <c r="S84" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="T84" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A85" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>37</v>
@@ -3688,131 +3694,131 @@
         <v>666</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J85" s="2">
         <v>0</v>
       </c>
       <c r="S85" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="T85" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A86" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J86" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="S86" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="T86" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A87" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I87" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="J87" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="S87" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="T87" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="J87" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="S87" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="T87" s="2" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A88" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J88" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="S88" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="T88" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A89" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>111</v>
       </c>
       <c r="G89" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="J89" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="L89" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="M89" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="H89" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="I89" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="J89" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="L89" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="M89" s="2" t="s">
-        <v>283</v>
-      </c>
       <c r="S89" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="T89" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A90" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>146</v>
@@ -3821,33 +3827,33 @@
         <v>0</v>
       </c>
       <c r="I90" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J90" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="L90" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="J90" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="L90" s="2" t="s">
+      <c r="M90" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="O90" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="M90" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="O90" s="2" t="s">
-        <v>217</v>
-      </c>
       <c r="P90" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="S90" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="T90" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A91" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>37</v>
@@ -3856,21 +3862,21 @@
         <v>1</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J91" s="2">
         <v>666</v>
       </c>
       <c r="S91" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="T91" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A92" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>37</v>
@@ -3879,21 +3885,21 @@
         <v>666</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J92" s="2">
         <v>1</v>
       </c>
       <c r="S92" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="T92" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="T92" s="2" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A93" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>37</v>
@@ -3902,76 +3908,76 @@
         <v>1</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J93" s="2">
         <v>1</v>
       </c>
       <c r="S93" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="T93" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A94" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G94" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H94" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="H94" s="2" t="s">
-        <v>225</v>
-      </c>
       <c r="I94" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J94" s="2">
         <v>888</v>
       </c>
       <c r="S94" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="T94" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A95" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E95" s="2">
         <v>2</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J95" s="2">
         <v>777</v>
       </c>
       <c r="L95" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M95" s="2">
         <v>777</v>
       </c>
       <c r="S95" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="T95" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A96" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>146</v>
@@ -3980,111 +3986,111 @@
         <v>2</v>
       </c>
       <c r="I96" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="J96" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="L96" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="M96" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="O96" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="J96" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="L96" s="2" t="s">
+      <c r="P96" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="S96" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="T96" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="M96" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="O96" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="P96" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="S96" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="T96" s="2" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A97" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="I97" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J97" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="S97" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="T97" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A98" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J98" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="S98" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="T98" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A99" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G99" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="I99" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="H99" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="I99" s="2" t="s">
-        <v>236</v>
-      </c>
       <c r="J99" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="S99" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="T99" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A100" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>146</v>
@@ -4093,33 +4099,33 @@
         <v>0</v>
       </c>
       <c r="I100" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="J100" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="L100" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="M100" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="O100" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="J100" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="L100" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="M100" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="O100" s="2" t="s">
+      <c r="P100" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="S100" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="P100" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="S100" s="2" t="s">
-        <v>236</v>
-      </c>
       <c r="T100" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A101" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>37</v>
@@ -4128,21 +4134,21 @@
         <v>0</v>
       </c>
       <c r="I101" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J101" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="S101" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="T101" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="102" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A102" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>37</v>
@@ -4151,21 +4157,21 @@
         <v>777</v>
       </c>
       <c r="I102" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="J102" s="2">
         <v>0</v>
       </c>
       <c r="S102" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="T102" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="103" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A103" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>37</v>
@@ -4174,21 +4180,21 @@
         <v>0</v>
       </c>
       <c r="I103" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J103" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="S103" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="T103" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A104" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>37</v>
@@ -4197,160 +4203,160 @@
         <v>777</v>
       </c>
       <c r="I104" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J104" s="2">
         <v>0</v>
       </c>
       <c r="S104" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="T104" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A105" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>111</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H105" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="J105" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="L105" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="M105" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="I105" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="J105" s="2" t="s">
+      <c r="S105" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="T105" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="L105" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="M105" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="S105" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="T105" s="2" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A106" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I106" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J106" s="2">
         <v>0</v>
       </c>
       <c r="S106" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="T106" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="107" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A107" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I107" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J107" s="2">
         <v>0</v>
       </c>
       <c r="S107" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="T107" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A108" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G108" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="H108" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I108" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="H108" s="2" t="s">
+      <c r="J108" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="I108" s="2" t="s">
+      <c r="S108" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="T108" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="J108" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="S108" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="T108" s="2" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="109" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A109" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E109" s="2">
         <v>0</v>
       </c>
       <c r="I109" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J109" s="2">
         <v>777</v>
       </c>
       <c r="L109" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="M109" s="2">
-        <v>7777</v>
+        <v>253</v>
+      </c>
+      <c r="M109" s="2" t="s">
+        <v>352</v>
       </c>
       <c r="S109" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="T109" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="110" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A110" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>34</v>
@@ -4362,15 +4368,15 @@
         <v>150</v>
       </c>
       <c r="S110" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="T110" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="111" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A111" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>34</v>
@@ -4382,24 +4388,24 @@
         <v>100</v>
       </c>
       <c r="S111" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="T111" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="112" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A112" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="I112" s="2" t="s">
         <v>25</v>
@@ -4408,24 +4414,24 @@
         <v>27</v>
       </c>
       <c r="S112" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="T112" s="2" t="s">
         <v>342</v>
-      </c>
-      <c r="T112" s="2" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="113" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A113" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I113" s="2" t="s">
         <v>25</v>
@@ -4434,24 +4440,24 @@
         <v>27</v>
       </c>
       <c r="S113" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="T113" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="114" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A114" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="I114" s="2" t="s">
         <v>25</v>
@@ -4460,10 +4466,10 @@
         <v>27</v>
       </c>
       <c r="S114" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="T114" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update V1 QC Core Warning Rules
</commit_message>
<xml_diff>
--- a/BCRPP_QC_R_Excel_Program/BCRPP_QC_DataDictionary_Version_1/Core QC Rules/BCRPP Warning Rules.xlsx
+++ b/BCRPP_QC_R_Excel_Program/BCRPP_QC_DataDictionary_Version_1/Core QC Rules/BCRPP Warning Rules.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28014"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A88CCA-E95C-4BF6-948A-EC450C4C0256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{FF3ECAE6-FA59-42D9-A401-5BC2971A3674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C71F37B-A02F-4CC5-9366-8D3BE64C24FD}"/>
   <bookViews>
     <workbookView xWindow="-76920" yWindow="-5820" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="353">
   <si>
     <t>Variable</t>
   </si>
@@ -179,7 +179,7 @@
     <t>birth_year</t>
   </si>
   <si>
-    <t>Verify: birth year is outside of range 1910-2010</t>
+    <t>Verify: birth year is outside of range 1900-2010</t>
   </si>
   <si>
     <t>sex</t>
@@ -230,6 +230,9 @@
     <t>agemenarche</t>
   </si>
   <si>
+    <t>Verify: agemenarche is outside of range 8-21 yrs</t>
+  </si>
+  <si>
     <t>height</t>
   </si>
   <si>
@@ -332,6 +335,18 @@
     <t>Verify: age_preg10 is outside range 12-58 years</t>
   </si>
   <si>
+    <t>Parity</t>
+  </si>
+  <si>
+    <t>1 &lt;= Parity &amp; Parity &lt; 15 | Parity == 888</t>
+  </si>
+  <si>
+    <t>parous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify Parity: Parous=1, but parity less than 1 or more than 15 pregnancies  </t>
+  </si>
+  <si>
     <t>parity</t>
   </si>
   <si>
@@ -341,40 +356,118 @@
     <t>age_preg2 != 666 &amp; age_preg1 != 666 &amp;  age_preg2 &gt; age_preg1 |age_preg1 == 888 | age_preg2 == 888</t>
   </si>
   <si>
+    <t>parity == 2 &amp; parity != 888 &amp; parity != 777</t>
+  </si>
+  <si>
+    <t>parity is 2, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
+  </si>
+  <si>
     <t>age_preg3,age_preg2,age_preg1</t>
   </si>
   <si>
+    <t>!age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666) &amp; age_preg3 &gt; age_preg2  | age_preg3 == 888 | age_preg2 == 888 | age_preg1 == 888</t>
+  </si>
+  <si>
+    <t>parity ==3 &amp; parity != 888 &amp; parity != 777</t>
+  </si>
+  <si>
+    <t>parity is 3, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
+  </si>
+  <si>
     <t>age_preg4,age_preg3,age_preg2,age_preg1</t>
   </si>
   <si>
+    <t>!age_preg4 %in% c(666) &amp; age_preg4 &gt; age_preg3 &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666)   | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 | age_preg1 == 888</t>
+  </si>
+  <si>
+    <t>parity ==4 &amp; parity != 888 &amp; parity != 777</t>
+  </si>
+  <si>
+    <t>parity is 4, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
+  </si>
+  <si>
     <t>age_preg5,age_preg4,age_preg3,age_preg2,age_preg1</t>
   </si>
   <si>
+    <t>!age_preg5 %in% c(666) &amp; age_preg5 &gt; age_preg4 &amp; !age_preg4 %in% c(666) &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666)  | age_preg5 == 888| age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 | age_preg1 == 888</t>
+  </si>
+  <si>
+    <t>parity ==5 &amp; parity != 888 &amp; parity != 777</t>
+  </si>
+  <si>
+    <t>parity is 5, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
+  </si>
+  <si>
     <t>age_preg6,age_preg5,age_preg4,age_preg3,age_preg2,age_preg1</t>
   </si>
   <si>
+    <t>!age_preg6 %in% c(666) &amp; age_preg6 &gt; age_preg5 &amp; !age_preg5 %in% c(666) &amp; !age_preg4 %in% c(666) &amp; !age_preg3 %in% c(666)&amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666) | age_preg6 == 888 | age_preg5 == 888 | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 | age_preg1 == 888</t>
+  </si>
+  <si>
+    <t>parity ==6 &amp; parity != 888 &amp; parity != 777</t>
+  </si>
+  <si>
+    <t>parity is 6, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
+  </si>
+  <si>
     <t>age_preg7,age_preg6,age_preg5,age_preg4,age_preg3,age_preg2,age_preg1</t>
   </si>
   <si>
+    <t>!age_preg7 %in% c(666) &amp; age_preg7 &gt; age_preg6 &amp; !age_preg6 %in% c(666)  &amp; !age_preg5 %in% c(666) &amp; !age_preg4  %in% c(666)  &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666) | age_preg7 == 888 | age_preg6 == 888 | age_preg5 == 888 | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 |age_preg1 == 888</t>
+  </si>
+  <si>
+    <t>parity ==7 &amp; parity != 888 &amp; parity != 777</t>
+  </si>
+  <si>
+    <t>parity is 7, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
+  </si>
+  <si>
     <t>age_preg8,age_preg7,age_preg6,age_preg5,age_preg4,age_preg3,age_preg2,age_preg1</t>
   </si>
   <si>
+    <t>!age_preg8 %in% c(666) &amp; age_preg8 &gt; age_preg7 &amp; !age_preg7 %in% c(666)  &amp; !age_preg6 %in% c(666) &amp; !age_preg5 %in% c(666)  &amp; !age_preg4 %in% c(666)  &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666)  | age_preg8 == 888 | age_preg7 == 888 | age_preg6 == 888 | age_preg5 == 888 | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 |age_preg1 == 888</t>
+  </si>
+  <si>
+    <t>parity ==8 &amp; parity != 888 &amp; parity != 777</t>
+  </si>
+  <si>
+    <t>parity is 8, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
+  </si>
+  <si>
     <t>age_preg9,age_preg8,age_preg7,age_preg6,age_preg5,age_preg4,age_preg3,age_preg2,age_preg1</t>
   </si>
   <si>
+    <t>!age_preg9 %in% c(666) &amp; age_preg9 &gt; age_preg8 &amp; !age_preg8 %in% c(666) &amp; !age_preg7 %in% c(666)  &amp; !age_preg6 %in% c(666) &amp; !age_preg5 %in% c(666) &amp; !age_preg4 %in% c(666) &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666) | age_preg9 == 888 | age_preg8 == 888 | age_preg7 == 888 | age_preg6 == 888 | age_preg5 == 888 | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 | age_preg1 == 888</t>
+  </si>
+  <si>
     <t xml:space="preserve">parity </t>
   </si>
   <si>
+    <t>parity ==9 &amp; parity != 888 &amp; parity != 777</t>
+  </si>
+  <si>
+    <t>parity is 9, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
+  </si>
+  <si>
     <t>age_preg10,age_preg9,age_preg8,age_preg7,age_preg6,age_preg5,age_preg4,age_preg3,age_preg2,age_preg1</t>
   </si>
   <si>
+    <t>!age_preg10 %in% c(666) &amp; age_preg10 &gt; age_preg9 &amp; !age_preg9 %in% c(666) &amp; !age_preg8 %in% c(666) &amp; !age_preg7 %in% c(666) &amp;  !age_preg6 %in% c(666)  &amp; !age_preg5 %in% c(666)  &amp; !age_preg4 %in% c(666) &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666)  | age_preg10 == 888 | age_preg9 == 888 | age_preg8 == 888 | age_preg7 == 888 | age_preg7 == 888 | age_preg6 == 888 | age_preg5 == 888 | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 | age_preg1 == 888</t>
+  </si>
+  <si>
+    <t>parity &gt;=10 &amp; parity != 888 &amp; parity != 777</t>
+  </si>
+  <si>
+    <t>parity is 10, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
+  </si>
+  <si>
     <t>breastfeed_dur_b1</t>
   </si>
   <si>
     <t>crossrange2.warnings</t>
   </si>
   <si>
-    <t>parous</t>
+    <t>breastfeed_dur_b1 &gt;= 0 &amp; breastfeed_dur_b1 &lt;= 24 | breastfeed_dur_b1 == 888 | breastfeed_dur_b1 == 666</t>
   </si>
   <si>
     <t>parous == 1</t>
@@ -389,6 +482,9 @@
     <t>breastfeed_dur_b2</t>
   </si>
   <si>
+    <t>breastfeed_dur_b2 &gt;= 0 &amp; breastfeed_dur_b2 &lt;= 24 | breastfeed_dur_b2 == 888 | breastfeed_dur_b2 == 666</t>
+  </si>
+  <si>
     <t xml:space="preserve">parity &gt;= 2   &amp; parity != 888  </t>
   </si>
   <si>
@@ -398,6 +494,9 @@
     <t>breastfeed_dur_b3</t>
   </si>
   <si>
+    <t>breastfeed_dur_b3 &gt;=0 &amp; breastfeed_dur_b3 &lt;= 24 | breastfeed_dur_b3 == 888 | breastfeed_dur_b3 == 666</t>
+  </si>
+  <si>
     <t xml:space="preserve">parity &gt;= 3  &amp; parity != 888  </t>
   </si>
   <si>
@@ -407,6 +506,9 @@
     <t>breastfeed_dur_b4</t>
   </si>
   <si>
+    <t>breastfeed_dur_b4 &gt;= 0 &amp; breastfeed_dur_b4 &lt;= 24| breastfeed_dur_b4 == 888 | breastfeed_dur_b4 == 666</t>
+  </si>
+  <si>
     <t xml:space="preserve">parity &gt;= 4  &amp; parity != 888  </t>
   </si>
   <si>
@@ -416,6 +518,9 @@
     <t>breastfeed_dur_b5</t>
   </si>
   <si>
+    <t>breastfeed_dur_b5 &gt;= 0 &amp; breastfeed_dur_b5 &lt;= 24 | breastfeed_dur_b5 == 888 | breastfeed_dur_b5 == 666</t>
+  </si>
+  <si>
     <t xml:space="preserve">parity &gt;= 5  &amp; parity != 888  </t>
   </si>
   <si>
@@ -425,6 +530,9 @@
     <t>breastfeed_dur_b6</t>
   </si>
   <si>
+    <t>breastfeed_dur_b6 &gt;= 0 &amp; breastfeed_dur_b6 &lt;= 24 | breastfeed_dur_b6 == 888 | breastfeed_dur_b6 == 666</t>
+  </si>
+  <si>
     <t xml:space="preserve">parity &gt;= 6  &amp; parity != 888  </t>
   </si>
   <si>
@@ -434,6 +542,9 @@
     <t>breastfeed_dur_b7</t>
   </si>
   <si>
+    <t>breastfeed_dur_b7 &gt;= 0 &amp; breastfeed_dur_b7 &lt;= 24 |  breastfeed_dur_b7 == 888 | breastfeed_dur_b7 == 666</t>
+  </si>
+  <si>
     <t xml:space="preserve">parity &gt;= 7  &amp; parity != 888  </t>
   </si>
   <si>
@@ -443,6 +554,9 @@
     <t>breastfeed_dur_b8</t>
   </si>
   <si>
+    <t>breastfeed_dur_b8 &gt;= 0 &amp; breastfeed_dur_b8 &lt;= 24 | breastfeed_dur_b8 == 888 | breastfeed_dur_b8 == 666</t>
+  </si>
+  <si>
     <t xml:space="preserve">parity &gt;= 8  &amp; parity != 888  </t>
   </si>
   <si>
@@ -452,6 +566,9 @@
     <t>breastfeed_dur_b9</t>
   </si>
   <si>
+    <t>breastfeed_dur_b9 &gt;= 0 &amp; breastfeed_dur_b9 &lt;= 24 | breastfeed_dur_b9 == 888 | breastfeed_dur_b9 == 666</t>
+  </si>
+  <si>
     <t xml:space="preserve">parity &gt;=9  &amp; parity != 888  </t>
   </si>
   <si>
@@ -461,6 +578,9 @@
     <t>breastfeed_dur_b10</t>
   </si>
   <si>
+    <t>breastfeed_dur_b10 &gt;= 0 &amp; breastfeed_dur_b10 &lt;= 24 | breastfeed_dur_b10 == 888 | breastfeed_dur_b10 == 666</t>
+  </si>
+  <si>
     <t xml:space="preserve">parity &gt;= 10  &amp; parity != 888  </t>
   </si>
   <si>
@@ -482,6 +602,9 @@
     <t>alcohol_init</t>
   </si>
   <si>
+    <t>777, 888</t>
+  </si>
+  <si>
     <t>alcohol_stop</t>
   </si>
   <si>
@@ -506,9 +629,15 @@
     <t>alcohol_init,age</t>
   </si>
   <si>
+    <t>alcohol_init &lt;= age</t>
+  </si>
+  <si>
     <t>!alcohol_init %in% c(777,888)</t>
   </si>
   <si>
+    <t>Verify: age at alcohol inititation (alcohol_init) is larger than the age at record date (age)</t>
+  </si>
+  <si>
     <t>2, 4</t>
   </si>
   <si>
@@ -518,6 +647,18 @@
     <t>alcohol_amt</t>
   </si>
   <si>
+    <t>alcohol_amt &gt; 0 &amp; alcohol_amt &lt; 42 | alcohol_amt == 888</t>
+  </si>
+  <si>
+    <t>Verify: alcohol_amt is outside range 0-42 gms</t>
+  </si>
+  <si>
+    <t>alcohol_stop &gt; 0 &amp; alcohol_stop &lt;= 100 | alcohol_stop ==888 | alcohol_stop == 666</t>
+  </si>
+  <si>
+    <t>!alcohol_status %in% c(1, 4, 888)</t>
+  </si>
+  <si>
     <t xml:space="preserve">alcohol_stop </t>
   </si>
   <si>
@@ -527,6 +668,9 @@
     <t>alcohol_dur &gt; 0 &amp; alcohol_dur &lt;= 50 | alcohol_dur == 888</t>
   </si>
   <si>
+    <t>!alcohol_status %in% c(4 ,888)</t>
+  </si>
+  <si>
     <t>Verify: alcohol_dur is outside range 0-50 years</t>
   </si>
   <si>
@@ -539,69 +683,90 @@
     <t>smoking_status</t>
   </si>
   <si>
+    <t>!smoking_status %in% c(4, 888)</t>
+  </si>
+  <si>
+    <t>Verify: smoking_init outside  range 0-70 years</t>
+  </si>
+  <si>
+    <t>smoking_amt</t>
+  </si>
+  <si>
+    <t>smoking_amt &gt; 0 &amp; smoking_amt &lt;= 60 | smoking_amt == 888</t>
+  </si>
+  <si>
+    <t>Verify: smoking_amt is outside  range 0-60 cigarrettes</t>
+  </si>
+  <si>
+    <t>smoking_amt %in% c(0,777, 888)</t>
+  </si>
+  <si>
+    <t>2, 3, 4</t>
+  </si>
+  <si>
+    <t>smoking_amt reflects current amount smoked, smoking_amt expected to be 0 or 777 if smoking_status is 2, 3, or 4</t>
+  </si>
+  <si>
+    <t>smoking_stop</t>
+  </si>
+  <si>
+    <t>smoking_stop &gt; 0 &amp; smoking_stop &lt;= 100 | smoking_stop == 888 | smoking_stop == 666</t>
+  </si>
+  <si>
+    <t>Verify: smoking_stop is outside range 0-100 years</t>
+  </si>
+  <si>
+    <t>smoking_dur</t>
+  </si>
+  <si>
+    <t>smoking_dur &gt;= 0 &amp; smoking_dur &lt;= 50 | smoking_dur ==888</t>
+  </si>
+  <si>
+    <t>smoking_stop != 666</t>
+  </si>
+  <si>
+    <t>Verify: smoking_dur is not within range 0-50 years</t>
+  </si>
+  <si>
+    <t>smoking_init,smoking_dur,smoking_stop</t>
+  </si>
+  <si>
+    <t>between(smoking_stop - smoking_init - smoking_dur, left = -2, right = 2)   | smoking_dur == 888</t>
+  </si>
+  <si>
+    <t>!smoking_init %in% c(777,888)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> !smoking_stop %in% c(666,777,888)</t>
+  </si>
+  <si>
+    <t>smoking_dur is more than the difference between smoking_init and smoking_stop ± 4 year window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">smoking_init </t>
+  </si>
+  <si>
+    <t>smoking_status is 4 (never smoker) ; not consistent with smoking_init, smoking_stop or smoking_dur</t>
+  </si>
+  <si>
+    <t>Verify: values of smoking_status and smoking_stop are not consistent</t>
+  </si>
+  <si>
+    <t>smoking_dur,age</t>
+  </si>
+  <si>
+    <t>smoking_dur &lt; age - 7 | smoking_dur == 888</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age </t>
+  </si>
+  <si>
+    <t>!is.na(age)</t>
+  </si>
+  <si>
     <t>!smoking_status %in% c(4,777,888)</t>
   </si>
   <si>
-    <t>Verify: smoking_init outside  range 0-70 years</t>
-  </si>
-  <si>
-    <t>smoking_amt</t>
-  </si>
-  <si>
-    <t>smoking_amt &gt; 0 &amp; smoking_amt &lt;= 60 | smoking_amt == 888</t>
-  </si>
-  <si>
-    <t>Verify: smoking_amt is outside  range 0-60 cigarrettes</t>
-  </si>
-  <si>
-    <t>smoking_stop</t>
-  </si>
-  <si>
-    <t>smoking_stop &gt; 0 &amp; smoking_stop &lt;= 100 | smoking_stop == 888 | smoking_stop == 666</t>
-  </si>
-  <si>
-    <t>Verify: smoking_stop is outside range 0-100 years</t>
-  </si>
-  <si>
-    <t>smoking_dur</t>
-  </si>
-  <si>
-    <t>smoking_stop != 666</t>
-  </si>
-  <si>
-    <t>Verify: smoking_dur is not within range 0-50 years</t>
-  </si>
-  <si>
-    <t>smoking_init,smoking_dur,smoking_stop</t>
-  </si>
-  <si>
-    <t>!smoking_init %in% c(777,888)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> !smoking_stop %in% c(666,777,888)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">smoking_init </t>
-  </si>
-  <si>
-    <t>smoking_status is 4 (never smoker) ; not consistent with smoking_init, smoking_stop or smoking_dur</t>
-  </si>
-  <si>
-    <t>Verify: values of smoking_status and smoking_stop are not consistent</t>
-  </si>
-  <si>
-    <t>smoking_dur,age</t>
-  </si>
-  <si>
-    <t>smoking_dur &lt; age - 7 | smoking_dur == 888</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age </t>
-  </si>
-  <si>
-    <t>!is.na(age)</t>
-  </si>
-  <si>
     <t>Verify: smoking_dur ≥ age - 7 years</t>
   </si>
   <si>
@@ -611,9 +776,15 @@
     <t>Biopsies_number</t>
   </si>
   <si>
+    <t>Biopsies_number != 0</t>
+  </si>
+  <si>
     <t>Verify: value of Biopsies_yesno = 1 not consistent with Biopsies_number</t>
   </si>
   <si>
+    <t>Biopsies_number == 0 | Biopsies_number == 888</t>
+  </si>
+  <si>
     <t>Verify: values of Biopsies_yesno = 0, not consistent with Biopsies_number</t>
   </si>
   <si>
@@ -629,9 +800,15 @@
     <t>BBD_number</t>
   </si>
   <si>
+    <t>BBD_number != 0</t>
+  </si>
+  <si>
     <t>Verify: BBD_history = 1, not consistent with BBD_number</t>
   </si>
   <si>
+    <t>0, 888</t>
+  </si>
+  <si>
     <t>Verify: BBD_history = 0, not consistent with BBD_number</t>
   </si>
   <si>
@@ -647,6 +824,9 @@
     <t>Verify: parous is 888, not consistent with age_preg1, parity, or breastfeed</t>
   </si>
   <si>
+    <t>!parity %in% c(0, 888)</t>
+  </si>
+  <si>
     <t>!breastfeed %in% c(777,888) &amp; !age_preg1 %in% c(777,888)</t>
   </si>
   <si>
@@ -674,18 +854,57 @@
     <t>ocuse_dur</t>
   </si>
   <si>
+    <t>ocuse_dur &gt; 0 &amp; ocuse_dur &lt;= 500 | ocuse_dur == 888</t>
+  </si>
+  <si>
     <t>ocuse_ever</t>
   </si>
   <si>
+    <t>!ocuse_ever %in% c(0,888)</t>
+  </si>
+  <si>
+    <t>Verify: ocuse_dur is outside range 0-500 months</t>
+  </si>
+  <si>
     <t>ocuse_start</t>
   </si>
   <si>
+    <t>ocuse_start &gt;= 10 &amp; ocuse_start &lt;= 58 | ocuse_start == 888</t>
+  </si>
+  <si>
     <t>Verify: ocuse_start is outside range 16-58 years</t>
   </si>
   <si>
     <t>ocuse_stop</t>
   </si>
   <si>
+    <t>ocuse_stop,ocuse_start</t>
+  </si>
+  <si>
+    <t>ocuse_stop &gt;= ocuse_start &amp; ocuse_stop &lt;= 58 | ocuse_stop == 888 | ocuse_stop == 666</t>
+  </si>
+  <si>
+    <t>Verify: ocuse_stop is either smaller than ocuse_start or greater than 58</t>
+  </si>
+  <si>
+    <t>ocuse_dur,ocuse_start,ocuse_stop</t>
+  </si>
+  <si>
+    <t>between(  (ocuse_stop * 12) - (ocuse_start * 12) - ocuse_dur, left = -24, right = 24)</t>
+  </si>
+  <si>
+    <t>!ocuse_start  %in% c(777,888)</t>
+  </si>
+  <si>
+    <t>!ocuse_stop %in% c(666, 777,888)</t>
+  </si>
+  <si>
+    <t>Verify: ocuse_dur is expected to be within the difference between ocuse_stop and ocuse_start ± 4 year window</t>
+  </si>
+  <si>
+    <t>0, 777, 888</t>
+  </si>
+  <si>
     <t>ocuse_ever is 0 (never user): not consistent with ocuse_start, or ocuse_stop, or ocuse_dur</t>
   </si>
   <si>
@@ -731,6 +950,9 @@
     <t>hrt_dur</t>
   </si>
   <si>
+    <t>666, 777</t>
+  </si>
+  <si>
     <t>hrtep_dur</t>
   </si>
   <si>
@@ -740,13 +962,37 @@
     <t>Verify:  verify values of hrt_dur, hrtep_dur, hrteonly_dur with meno_status = 2 (pre-menopausal)</t>
   </si>
   <si>
+    <t>hrt_dur &gt; 0 &amp; hrt_dur &lt;= 300 | hrt_dur == 888 | hrt_dur == 666</t>
+  </si>
+  <si>
     <t>hrtuse</t>
   </si>
   <si>
     <t>!hrtuse %in% c(0,888)</t>
   </si>
   <si>
-    <t>666, 777</t>
+    <t>Verify: hrt_dur is outside range 0-300 months</t>
+  </si>
+  <si>
+    <t>hrtep_dur &gt; 0 &amp; hrtep_dur &lt;= 300 | hrtep_dur == 888 | hrtep_dur == 666</t>
+  </si>
+  <si>
+    <t>!hrtuse_ep %in% c(0,888)</t>
+  </si>
+  <si>
+    <t>Verify: hrtep_dur is outside range 0-300 months</t>
+  </si>
+  <si>
+    <t>hrteonly_dur &gt; 0 &amp; hrteonly_dur &lt;= 300 | hrteonly_dur == 888 | hrteonly_dur == 666</t>
+  </si>
+  <si>
+    <t>!hrtuse_eonly %in% c(0,888)</t>
+  </si>
+  <si>
+    <t>Verify: hrteonly_dur is outside range 0-300 months</t>
+  </si>
+  <si>
+    <t>666, 777, 888</t>
   </si>
   <si>
     <t xml:space="preserve">hrtuse is 0 (never user):  not consistent with hrt_dur, hrtep_dur, or hrteonly_dur </t>
@@ -758,12 +1004,18 @@
     <t>Verify:  hrtuse_ep is 0 (never user), not consistent with hrtep_dur</t>
   </si>
   <si>
+    <t>Verify: hrtep_dur is 777, not consistent with hrtuse_ep</t>
+  </si>
+  <si>
     <t>hrtuse_eonly</t>
   </si>
   <si>
     <t>hrtuse_eonly is 0 ( never user) but hrteonly_dur is not 666 or777</t>
   </si>
   <si>
+    <t>hrteonly_dur is  777  hrtuse_eonly should be 0</t>
+  </si>
+  <si>
     <t>hrtuse == 1</t>
   </si>
   <si>
@@ -776,9 +1028,15 @@
     <t>hrtuse is not 1 but hrtuse_eonly and hrtuse_ep are 1 (current user)</t>
   </si>
   <si>
+    <t>hrtuse_ep == 0 | hrtuse_ep == 888</t>
+  </si>
+  <si>
     <t>hrtuse is 0 (never user), not consistent with hrtuse_eponly</t>
   </si>
   <si>
+    <t>hrtuse_eonly == 0 | hrtuse_eonly == 888</t>
+  </si>
+  <si>
     <t>hrtuse is 0 (never user), not consistent with hrtuse_eonly</t>
   </si>
   <si>
@@ -800,264 +1058,24 @@
     <t>lastscreen_year</t>
   </si>
   <si>
+    <t>777, 7777</t>
+  </si>
+  <si>
     <t xml:space="preserve">screen_ever is 0, not consistent with lastscreen_year or screen_start </t>
   </si>
   <si>
     <t>pa_mets</t>
   </si>
   <si>
+    <t>Verify: pa_mets is not within range 0-150 METS</t>
+  </si>
+  <si>
     <t>pa_pct</t>
   </si>
   <si>
     <t>pa_pct is not within range 0-100 %</t>
   </si>
   <si>
-    <t>alcohol_init &lt;= age</t>
-  </si>
-  <si>
-    <t>Verify: age at alcohol inititation (alcohol_init) is larger than the age at record date (age)</t>
-  </si>
-  <si>
-    <t>!alcohol_status %in% c(1, 4, 888)</t>
-  </si>
-  <si>
-    <t>!alcohol_status %in% c(4 ,888)</t>
-  </si>
-  <si>
-    <t>alcohol_stop &gt; 0 &amp; alcohol_stop &lt;= 100 | alcohol_stop ==888 | alcohol_stop == 666</t>
-  </si>
-  <si>
-    <t>!smoking_status %in% c(4, 888)</t>
-  </si>
-  <si>
-    <t>!parity %in% c(0, 888)</t>
-  </si>
-  <si>
-    <t>breastfeed_dur_b1 &gt;= 0 &amp; breastfeed_dur_b1 &lt;= 24 | breastfeed_dur_b1 == 888 | breastfeed_dur_b1 == 666</t>
-  </si>
-  <si>
-    <t>breastfeed_dur_b2 &gt;= 0 &amp; breastfeed_dur_b2 &lt;= 24 | breastfeed_dur_b2 == 888 | breastfeed_dur_b2 == 666</t>
-  </si>
-  <si>
-    <t>breastfeed_dur_b3 &gt;=0 &amp; breastfeed_dur_b3 &lt;= 24 | breastfeed_dur_b3 == 888 | breastfeed_dur_b3 == 666</t>
-  </si>
-  <si>
-    <t>breastfeed_dur_b4 &gt;= 0 &amp; breastfeed_dur_b4 &lt;= 24| breastfeed_dur_b4 == 888 | breastfeed_dur_b4 == 666</t>
-  </si>
-  <si>
-    <t>breastfeed_dur_b5 &gt;= 0 &amp; breastfeed_dur_b5 &lt;= 24 | breastfeed_dur_b5 == 888 | breastfeed_dur_b5 == 666</t>
-  </si>
-  <si>
-    <t>breastfeed_dur_b6 &gt;= 0 &amp; breastfeed_dur_b6 &lt;= 24 | breastfeed_dur_b6 == 888 | breastfeed_dur_b6 == 666</t>
-  </si>
-  <si>
-    <t>breastfeed_dur_b7 &gt;= 0 &amp; breastfeed_dur_b7 &lt;= 24 |  breastfeed_dur_b7 == 888 | breastfeed_dur_b7 == 666</t>
-  </si>
-  <si>
-    <t>breastfeed_dur_b8 &gt;= 0 &amp; breastfeed_dur_b8 &lt;= 24 | breastfeed_dur_b8 == 888 | breastfeed_dur_b8 == 666</t>
-  </si>
-  <si>
-    <t>breastfeed_dur_b9 &gt;= 0 &amp; breastfeed_dur_b9 &lt;= 24 | breastfeed_dur_b9 == 888 | breastfeed_dur_b9 == 666</t>
-  </si>
-  <si>
-    <t>breastfeed_dur_b10 &gt;= 0 &amp; breastfeed_dur_b10 &lt;= 24 | breastfeed_dur_b10 == 888 | breastfeed_dur_b10 == 666</t>
-  </si>
-  <si>
-    <t>ocuse_dur &gt; 0 &amp; ocuse_dur &lt;= 500 | ocuse_dur == 888</t>
-  </si>
-  <si>
-    <t>!ocuse_ever %in% c(0,888)</t>
-  </si>
-  <si>
-    <t>ocuse_start &gt;= 10 &amp; ocuse_start &lt;= 58 | ocuse_start == 888</t>
-  </si>
-  <si>
-    <t>ocuse_stop,ocuse_start</t>
-  </si>
-  <si>
-    <t>ocuse_dur,ocuse_start,ocuse_stop</t>
-  </si>
-  <si>
-    <t>!ocuse_start  %in% c(777,888)</t>
-  </si>
-  <si>
-    <t>!ocuse_stop %in% c(666, 777,888)</t>
-  </si>
-  <si>
-    <t>Verify: hrt_dur is outside range 0-300 months</t>
-  </si>
-  <si>
-    <t>Verify: hrtep_dur is outside range 0-300 months</t>
-  </si>
-  <si>
-    <t>Verify: hrteonly_dur is outside range 0-300 months</t>
-  </si>
-  <si>
-    <t>Verify: hrtep_dur is 777, not consistent with hrtuse_ep</t>
-  </si>
-  <si>
-    <t>hrteonly_dur is  777  hrtuse_eonly should be 0</t>
-  </si>
-  <si>
-    <t>Verify: pa_mets is not within range 0-150 METS</t>
-  </si>
-  <si>
-    <t>2, 3, 4</t>
-  </si>
-  <si>
-    <t>Verify: ocuse_dur is outside range 0-500 months</t>
-  </si>
-  <si>
-    <t>!hrtuse_ep %in% c(0,888)</t>
-  </si>
-  <si>
-    <t>!hrtuse_eonly %in% c(0,888)</t>
-  </si>
-  <si>
-    <t>smoking_amt %in% c(0,777, 888)</t>
-  </si>
-  <si>
-    <t>777, 888</t>
-  </si>
-  <si>
-    <t>0, 888</t>
-  </si>
-  <si>
-    <t>0, 777, 888</t>
-  </si>
-  <si>
-    <t>666, 777, 888</t>
-  </si>
-  <si>
-    <t>hrtuse_ep == 0 | hrtuse_ep == 888</t>
-  </si>
-  <si>
-    <t>hrtuse_eonly == 0 | hrtuse_eonly == 888</t>
-  </si>
-  <si>
-    <t>Biopsies_number == 0 | Biopsies_number == 888</t>
-  </si>
-  <si>
-    <t>BBD_number != 0</t>
-  </si>
-  <si>
-    <t>Biopsies_number != 0</t>
-  </si>
-  <si>
-    <t>smoking_amt reflects current amount smoked, smoking_amt expected to be 0 or 777 if smoking_status is 2, 3, or 4</t>
-  </si>
-  <si>
-    <t>smoking_dur is more than the difference between smoking_init and smoking_stop ± 4 year window</t>
-  </si>
-  <si>
-    <t>between(smoking_stop - smoking_init - smoking_dur, left = -2, right = 2)   | smoking_dur == 888</t>
-  </si>
-  <si>
-    <t>between(  (ocuse_stop * 12) - (ocuse_start * 12) - ocuse_dur, left = -24, right = 24)</t>
-  </si>
-  <si>
-    <t>Verify: ocuse_dur is expected to be within the difference between ocuse_stop and ocuse_start ± 4 year window</t>
-  </si>
-  <si>
-    <t>Verify: ocuse_stop is either smaller than ocuse_start or greater than 58</t>
-  </si>
-  <si>
-    <t>ocuse_stop &gt;= ocuse_start &amp; ocuse_stop &lt;= 58 | ocuse_stop == 888 | ocuse_stop == 666</t>
-  </si>
-  <si>
-    <t>Verify: agemenarche is outside of range 8-21 yrs</t>
-  </si>
-  <si>
-    <t>parity == 2 &amp; parity != 888 &amp; parity != 777</t>
-  </si>
-  <si>
-    <t>parity ==3 &amp; parity != 888 &amp; parity != 777</t>
-  </si>
-  <si>
-    <t>parity ==4 &amp; parity != 888 &amp; parity != 777</t>
-  </si>
-  <si>
-    <t>parity ==5 &amp; parity != 888 &amp; parity != 777</t>
-  </si>
-  <si>
-    <t>parity ==6 &amp; parity != 888 &amp; parity != 777</t>
-  </si>
-  <si>
-    <t>parity ==7 &amp; parity != 888 &amp; parity != 777</t>
-  </si>
-  <si>
-    <t>parity ==8 &amp; parity != 888 &amp; parity != 777</t>
-  </si>
-  <si>
-    <t>parity ==9 &amp; parity != 888 &amp; parity != 777</t>
-  </si>
-  <si>
-    <t>parity is 2, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
-  </si>
-  <si>
-    <t>parity is 3, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
-  </si>
-  <si>
-    <t>parity is 5, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
-  </si>
-  <si>
-    <t>parity is 6, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
-  </si>
-  <si>
-    <t>parity is 8, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
-  </si>
-  <si>
-    <t>parity is 10, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
-  </si>
-  <si>
-    <t>parity is 9, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
-  </si>
-  <si>
-    <t>parity is 7, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
-  </si>
-  <si>
-    <t>parity is 4, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
-  </si>
-  <si>
-    <t>!age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666) &amp; age_preg3 &gt; age_preg2  | age_preg3 == 888 | age_preg2 == 888 | age_preg1 == 888</t>
-  </si>
-  <si>
-    <t>!age_preg4 %in% c(666) &amp; age_preg4 &gt; age_preg3 &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666)   | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 | age_preg1 == 888</t>
-  </si>
-  <si>
-    <t>!age_preg6 %in% c(666) &amp; age_preg6 &gt; age_preg5 &amp; !age_preg5 %in% c(666) &amp; !age_preg4 %in% c(666) &amp; !age_preg3 %in% c(666)&amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666) | age_preg6 == 888 | age_preg5 == 888 | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 | age_preg1 == 888</t>
-  </si>
-  <si>
-    <t>!age_preg7 %in% c(666) &amp; age_preg7 &gt; age_preg6 &amp; !age_preg6 %in% c(666)  &amp; !age_preg5 %in% c(666) &amp; !age_preg4  %in% c(666)  &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666) | age_preg7 == 888 | age_preg6 == 888 | age_preg5 == 888 | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 |age_preg1 == 888</t>
-  </si>
-  <si>
-    <t>!age_preg8 %in% c(666) &amp; age_preg8 &gt; age_preg7 &amp; !age_preg7 %in% c(666)  &amp; !age_preg6 %in% c(666) &amp; !age_preg5 %in% c(666)  &amp; !age_preg4 %in% c(666)  &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666)  | age_preg8 == 888 | age_preg7 == 888 | age_preg6 == 888 | age_preg5 == 888 | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 |age_preg1 == 888</t>
-  </si>
-  <si>
-    <t>!age_preg9 %in% c(666) &amp; age_preg9 &gt; age_preg8 &amp; !age_preg8 %in% c(666) &amp; !age_preg7 %in% c(666)  &amp; !age_preg6 %in% c(666) &amp; !age_preg5 %in% c(666) &amp; !age_preg4 %in% c(666) &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666) | age_preg9 == 888 | age_preg8 == 888 | age_preg7 == 888 | age_preg6 == 888 | age_preg5 == 888 | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 | age_preg1 == 888</t>
-  </si>
-  <si>
-    <t>!age_preg10 %in% c(666) &amp; age_preg10 &gt; age_preg9 &amp; !age_preg9 %in% c(666) &amp; !age_preg8 %in% c(666) &amp; !age_preg7 %in% c(666) &amp;  !age_preg6 %in% c(666)  &amp; !age_preg5 %in% c(666)  &amp; !age_preg4 %in% c(666) &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666)  | age_preg10 == 888 | age_preg9 == 888 | age_preg8 == 888 | age_preg7 == 888 | age_preg7 == 888 | age_preg6 == 888 | age_preg5 == 888 | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 | age_preg1 == 888</t>
-  </si>
-  <si>
-    <t>parity &gt;=10 &amp; parity != 888 &amp; parity != 777</t>
-  </si>
-  <si>
-    <t>!age_preg5 %in% c(666) &amp; age_preg5 &gt; age_preg4 &amp; !age_preg4 %in% c(666) &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666)  | age_preg5 == 888| age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 | age_preg1 == 888</t>
-  </si>
-  <si>
-    <t>smoking_dur &gt;= 0 &amp; smoking_dur &lt;= 50 | smoking_dur ==888</t>
-  </si>
-  <si>
-    <t>hrtep_dur &gt; 0 &amp; hrtep_dur &lt;= 300 | hrtep_dur == 888 | hrtep_dur == 666</t>
-  </si>
-  <si>
-    <t>hrteonly_dur &gt; 0 &amp; hrteonly_dur &lt;= 300 | hrteonly_dur == 888 | hrteonly_dur == 666</t>
-  </si>
-  <si>
-    <t>hrt_dur &gt; 0 &amp; hrt_dur &lt;= 300 | hrt_dur == 888 | hrt_dur == 666</t>
-  </si>
-  <si>
     <t>lastfup</t>
   </si>
   <si>
@@ -1077,31 +1095,13 @@
   </si>
   <si>
     <t>Please provide an explanation for why lastfup is missing/unknown.</t>
-  </si>
-  <si>
-    <t>Parity</t>
-  </si>
-  <si>
-    <t>1 &lt;= Parity &amp; Parity &lt; 15 | Parity == 888</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify Parity: Parous=1, but parity less than 1 or more than 15 pregnancies  </t>
-  </si>
-  <si>
-    <t>alcohol_amt &gt; 0 &amp; alcohol_amt &lt; 42 | alcohol_amt == 888</t>
-  </si>
-  <si>
-    <t>Verify: alcohol_amt is outside range 0-42 gms</t>
-  </si>
-  <si>
-    <t>777, 7777</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1470,38 +1470,38 @@
   <dimension ref="A1:U114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I93" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="B56" sqref="B56"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M109" sqref="M109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.600000000000001"/>
   <cols>
-    <col min="1" max="1" width="24.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="119.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="255.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="45.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="64.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="119.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="255.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="64.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="180" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.81640625" style="2"/>
+    <col min="21" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:20">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:20">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:20">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:20">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:20">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:20">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:20">
       <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:20">
       <c r="A9" s="2" t="s">
         <v>43</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:20">
       <c r="A10" s="2" t="s">
         <v>46</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>34</v>
       </c>
       <c r="C10" s="2">
-        <v>1910</v>
+        <v>1900</v>
       </c>
       <c r="D10" s="2">
         <v>2010</v>
@@ -1761,7 +1761,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:20">
       <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:20">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:20">
       <c r="A13" s="2" t="s">
         <v>53</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:20">
       <c r="A14" s="2" t="s">
         <v>56</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:20">
       <c r="A15" s="2" t="s">
         <v>58</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:20">
       <c r="A16" s="2" t="s">
         <v>61</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:20">
       <c r="A17" s="2" t="s">
         <v>63</v>
       </c>
@@ -1883,12 +1883,12 @@
         <v>63</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.45">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
       <c r="A18" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>34</v>
@@ -1900,15 +1900,15 @@
         <v>200</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.45">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
       <c r="A19" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>34</v>
@@ -1920,15 +1920,15 @@
         <v>50</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.45">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
       <c r="A20" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>34</v>
@@ -1940,15 +1940,15 @@
         <v>150</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
       <c r="A21" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>34</v>
@@ -1960,15 +1960,15 @@
         <v>50</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
       <c r="A22" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>34</v>
@@ -1980,15 +1980,15 @@
         <v>160</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.45">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
       <c r="A23" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>34</v>
@@ -2000,15 +2000,15 @@
         <v>160</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
       <c r="A24" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>34</v>
@@ -2020,15 +2020,15 @@
         <v>1.2</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.45">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
       <c r="A25" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>34</v>
@@ -2040,15 +2040,15 @@
         <v>58</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="T25" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.45">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
       <c r="A26" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>34</v>
@@ -2060,15 +2060,15 @@
         <v>58</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="T26" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.45">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
       <c r="A27" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>34</v>
@@ -2080,15 +2080,15 @@
         <v>58</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="T27" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.45">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
       <c r="A28" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>34</v>
@@ -2100,15 +2100,15 @@
         <v>58</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="T28" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.45">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20">
       <c r="A29" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>34</v>
@@ -2120,15 +2120,15 @@
         <v>58</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="T29" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.45">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
       <c r="A30" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>34</v>
@@ -2140,15 +2140,15 @@
         <v>58</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="T30" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
       <c r="A31" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>34</v>
@@ -2160,15 +2160,15 @@
         <v>58</v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="T31" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.45">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20">
       <c r="A32" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>34</v>
@@ -2180,15 +2180,15 @@
         <v>58</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="T32" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.45">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
       <c r="A33" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>34</v>
@@ -2200,15 +2200,15 @@
         <v>58</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="T33" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.45">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
       <c r="A34" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>34</v>
@@ -2220,15 +2220,15 @@
         <v>58</v>
       </c>
       <c r="S34" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="T34" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.45">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21">
       <c r="A35" s="3" t="s">
-        <v>347</v>
+        <v>99</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>21</v>
@@ -2238,13 +2238,13 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3" t="s">
-        <v>347</v>
+        <v>99</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>348</v>
+        <v>100</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="J35" s="3">
         <v>1</v>
@@ -2258,253 +2258,253 @@
       <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
       <c r="S35" s="3" t="s">
-        <v>347</v>
+        <v>99</v>
       </c>
       <c r="T35" s="3" t="s">
-        <v>349</v>
+        <v>102</v>
       </c>
       <c r="U35" s="3"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:21">
       <c r="A36" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>310</v>
+        <v>106</v>
       </c>
       <c r="S36" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="T36" s="2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.45">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21">
       <c r="A37" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>327</v>
+        <v>109</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>311</v>
+        <v>110</v>
       </c>
       <c r="S37" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="T37" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.45">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21">
       <c r="A38" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>328</v>
+        <v>113</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>312</v>
+        <v>114</v>
       </c>
       <c r="S38" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="T38" s="2" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.45">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
       <c r="A39" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G39" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I39" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="H39" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="J39" s="2" t="s">
-        <v>313</v>
+        <v>118</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="T39" s="3" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21">
       <c r="A40" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>329</v>
+        <v>121</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>314</v>
+        <v>122</v>
       </c>
       <c r="S40" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="T40" s="3" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.45">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21">
       <c r="A41" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>330</v>
+        <v>125</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>315</v>
+        <v>126</v>
       </c>
       <c r="S41" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="T41" s="3" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.45">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21">
       <c r="A42" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>331</v>
+        <v>129</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>316</v>
+        <v>130</v>
       </c>
       <c r="S42" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="T42" s="3" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21">
       <c r="A43" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>332</v>
+        <v>133</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>317</v>
+        <v>135</v>
       </c>
       <c r="S43" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="T43" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.45">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21">
       <c r="A44" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>109</v>
+        <v>137</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>333</v>
+        <v>138</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>334</v>
+        <v>139</v>
       </c>
       <c r="S44" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="T44" s="3" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.45">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21">
       <c r="A45" s="2" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="C45" s="2">
         <v>0</v>
@@ -2513,36 +2513,36 @@
         <v>24</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>265</v>
+        <v>143</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>114</v>
+        <v>145</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="T45" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.45">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21">
       <c r="A46" s="2" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="C46" s="2">
         <v>0</v>
@@ -2551,36 +2551,36 @@
         <v>24</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>266</v>
+        <v>148</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="S46" s="2" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="T46" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.45">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21">
       <c r="A47" s="2" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="C47" s="2">
         <v>0</v>
@@ -2589,36 +2589,36 @@
         <v>24</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>267</v>
+        <v>152</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>120</v>
+        <v>153</v>
       </c>
       <c r="S47" s="2" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
       <c r="T47" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.45">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21">
       <c r="A48" s="2" t="s">
-        <v>122</v>
+        <v>155</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="C48" s="2">
         <v>0</v>
@@ -2627,36 +2627,36 @@
         <v>24</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>122</v>
+        <v>155</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>268</v>
+        <v>156</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="S48" s="3" t="s">
-        <v>122</v>
+        <v>155</v>
       </c>
       <c r="T48" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.45">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20">
       <c r="A49" s="2" t="s">
-        <v>125</v>
+        <v>159</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="C49" s="2">
         <v>0</v>
@@ -2665,36 +2665,36 @@
         <v>24</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>125</v>
+        <v>159</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>269</v>
+        <v>160</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
       <c r="S49" s="3" t="s">
-        <v>125</v>
+        <v>159</v>
       </c>
       <c r="T49" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.45">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20">
       <c r="A50" s="2" t="s">
-        <v>128</v>
+        <v>163</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="C50" s="2">
         <v>0</v>
@@ -2703,36 +2703,36 @@
         <v>24</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>128</v>
+        <v>163</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>270</v>
+        <v>164</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>129</v>
+        <v>165</v>
       </c>
       <c r="S50" s="3" t="s">
-        <v>128</v>
+        <v>163</v>
       </c>
       <c r="T50" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.45">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20">
       <c r="A51" s="2" t="s">
-        <v>131</v>
+        <v>167</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="C51" s="2">
         <v>0</v>
@@ -2741,36 +2741,36 @@
         <v>24</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>131</v>
+        <v>167</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>271</v>
+        <v>168</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>132</v>
+        <v>169</v>
       </c>
       <c r="S51" s="2" t="s">
-        <v>131</v>
+        <v>167</v>
       </c>
       <c r="T51" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.45">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20">
       <c r="A52" s="2" t="s">
-        <v>134</v>
+        <v>171</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="C52" s="2">
         <v>0</v>
@@ -2779,36 +2779,36 @@
         <v>24</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>134</v>
+        <v>171</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>272</v>
+        <v>172</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>135</v>
+        <v>173</v>
       </c>
       <c r="S52" s="3" t="s">
-        <v>134</v>
+        <v>171</v>
       </c>
       <c r="T52" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.45">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20">
       <c r="A53" s="2" t="s">
-        <v>137</v>
+        <v>175</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="C53" s="2">
         <v>0</v>
@@ -2817,36 +2817,36 @@
         <v>24</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>137</v>
+        <v>175</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>273</v>
+        <v>176</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>138</v>
+        <v>177</v>
       </c>
       <c r="S53" s="3" t="s">
-        <v>137</v>
+        <v>175</v>
       </c>
       <c r="T53" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.45">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20">
       <c r="A54" s="2" t="s">
-        <v>140</v>
+        <v>179</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="C54" s="2">
         <v>0</v>
@@ -2855,85 +2855,85 @@
         <v>24</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>140</v>
+        <v>179</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>274</v>
+        <v>180</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>141</v>
+        <v>181</v>
       </c>
       <c r="S54" s="2" t="s">
-        <v>140</v>
+        <v>179</v>
       </c>
       <c r="T54" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.45">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20">
       <c r="A55" s="2" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>144</v>
+        <v>184</v>
       </c>
       <c r="S55" s="2" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="T55" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.45">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20">
       <c r="A56" s="2" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="E56" s="2">
         <v>4</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="J56" s="2">
-        <v>777</v>
+        <v>187</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="M56" s="2">
-        <v>777</v>
+        <v>189</v>
+      </c>
+      <c r="M56" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="O56" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="P56" s="2">
-        <v>777</v>
+        <v>190</v>
+      </c>
+      <c r="P56" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="S56" s="2" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="T56" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.45">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20">
       <c r="A57" s="2" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>37</v>
@@ -2942,73 +2942,73 @@
         <v>1</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>148</v>
+        <v>189</v>
       </c>
       <c r="J57" s="2">
         <v>666</v>
       </c>
       <c r="S57" s="2" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="T57" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.45">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20">
       <c r="A58" s="2" t="s">
-        <v>147</v>
+        <v>187</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>147</v>
+        <v>187</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>152</v>
+        <v>193</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>153</v>
+        <v>194</v>
       </c>
       <c r="S58" s="2" t="s">
-        <v>147</v>
+        <v>187</v>
       </c>
       <c r="T58" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.45">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20">
       <c r="A59" s="2" t="s">
-        <v>147</v>
+        <v>187</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>155</v>
+        <v>196</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>258</v>
+        <v>197</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>147</v>
+        <v>187</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>156</v>
+        <v>198</v>
       </c>
       <c r="S59" s="2" t="s">
-        <v>147</v>
+        <v>187</v>
       </c>
       <c r="T59" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.45">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20">
       <c r="A60" s="2" t="s">
-        <v>147</v>
+        <v>187</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>37</v>
@@ -3017,302 +3017,302 @@
         <v>777</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>157</v>
+        <v>200</v>
       </c>
       <c r="S60" s="2" t="s">
-        <v>147</v>
+        <v>187</v>
       </c>
       <c r="T60" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.45">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20">
       <c r="A61" s="2" t="s">
-        <v>159</v>
+        <v>202</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>159</v>
+        <v>202</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>350</v>
+        <v>203</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="J61" s="2">
         <v>1</v>
       </c>
       <c r="S61" s="2" t="s">
-        <v>159</v>
+        <v>202</v>
       </c>
       <c r="T61" s="2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.45">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20">
       <c r="A62" s="2" t="s">
-        <v>148</v>
+        <v>189</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>148</v>
+        <v>189</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>262</v>
+        <v>205</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>260</v>
+        <v>206</v>
       </c>
       <c r="S62" s="2" t="s">
-        <v>160</v>
+        <v>207</v>
       </c>
       <c r="T62" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.45">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20">
       <c r="A63" s="2" t="s">
-        <v>149</v>
+        <v>190</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>149</v>
+        <v>190</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>162</v>
+        <v>209</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>261</v>
+        <v>210</v>
       </c>
       <c r="S63" s="2" t="s">
-        <v>149</v>
+        <v>190</v>
       </c>
       <c r="T63" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.45">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20">
       <c r="A64" s="2" t="s">
-        <v>164</v>
+        <v>212</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>164</v>
+        <v>212</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>165</v>
+        <v>213</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>166</v>
+        <v>214</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>263</v>
+        <v>215</v>
       </c>
       <c r="S64" s="2" t="s">
-        <v>164</v>
+        <v>212</v>
       </c>
       <c r="T64" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.45">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20">
       <c r="A65" s="2" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>170</v>
+        <v>218</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>166</v>
+        <v>214</v>
       </c>
       <c r="J65" s="2">
         <v>1</v>
       </c>
       <c r="S65" s="2" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
       <c r="T65" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.45">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20">
       <c r="A66" s="2" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>292</v>
+        <v>220</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>166</v>
+        <v>214</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>288</v>
+        <v>221</v>
       </c>
       <c r="S66" s="2" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
       <c r="T66" s="2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.45">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20">
       <c r="A67" s="2" t="s">
-        <v>172</v>
+        <v>223</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>172</v>
+        <v>223</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>173</v>
+        <v>224</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>166</v>
+        <v>214</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>263</v>
+        <v>215</v>
       </c>
       <c r="S67" s="2" t="s">
-        <v>172</v>
+        <v>223</v>
       </c>
       <c r="T67" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.45">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20">
       <c r="A68" s="2" t="s">
-        <v>175</v>
+        <v>226</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>175</v>
+        <v>226</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>336</v>
+        <v>227</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>166</v>
+        <v>214</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>263</v>
+        <v>215</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>172</v>
+        <v>223</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>176</v>
+        <v>228</v>
       </c>
       <c r="S68" s="2" t="s">
-        <v>175</v>
+        <v>226</v>
       </c>
       <c r="T68" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.45">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20">
       <c r="A69" s="2" t="s">
-        <v>175</v>
+        <v>226</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>178</v>
+        <v>230</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>304</v>
+        <v>231</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>164</v>
+        <v>212</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>179</v>
+        <v>232</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>172</v>
+        <v>223</v>
       </c>
       <c r="M69" s="2" t="s">
-        <v>180</v>
+        <v>233</v>
       </c>
       <c r="S69" s="2" t="s">
-        <v>175</v>
+        <v>226</v>
       </c>
       <c r="T69" s="2" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.45">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20">
       <c r="A70" s="2" t="s">
-        <v>166</v>
+        <v>214</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="E70" s="2">
         <v>4</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>181</v>
+        <v>235</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>293</v>
+        <v>188</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>172</v>
+        <v>223</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>293</v>
+        <v>188</v>
       </c>
       <c r="O70" s="2" t="s">
-        <v>175</v>
+        <v>226</v>
       </c>
       <c r="P70" s="2" t="s">
-        <v>293</v>
+        <v>188</v>
       </c>
       <c r="S70" s="2" t="s">
-        <v>166</v>
+        <v>214</v>
       </c>
       <c r="T70" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.45">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20">
       <c r="A71" s="2" t="s">
-        <v>166</v>
+        <v>214</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>37</v>
@@ -3321,157 +3321,157 @@
         <v>1</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>172</v>
+        <v>223</v>
       </c>
       <c r="J71" s="2">
         <v>666</v>
       </c>
       <c r="S71" s="2" t="s">
-        <v>166</v>
+        <v>214</v>
       </c>
       <c r="T71" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.45">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20">
       <c r="A72" s="2" t="s">
-        <v>175</v>
+        <v>226</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>184</v>
+        <v>238</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>185</v>
+        <v>239</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>186</v>
+        <v>240</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>187</v>
+        <v>241</v>
       </c>
       <c r="L72" s="2" t="s">
-        <v>166</v>
+        <v>214</v>
       </c>
       <c r="M72" s="2" t="s">
-        <v>167</v>
+        <v>242</v>
       </c>
       <c r="S72" s="2" t="s">
-        <v>175</v>
+        <v>226</v>
       </c>
       <c r="T72" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.45">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20">
       <c r="A73" s="2" t="s">
-        <v>189</v>
+        <v>244</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>190</v>
+        <v>245</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>301</v>
+        <v>246</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>189</v>
+        <v>244</v>
       </c>
       <c r="J73" s="2">
         <v>1</v>
       </c>
       <c r="S73" s="2" t="s">
-        <v>190</v>
+        <v>245</v>
       </c>
       <c r="T73" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.45">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20">
       <c r="A74" s="2" t="s">
-        <v>189</v>
+        <v>244</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>190</v>
+        <v>245</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>299</v>
+        <v>248</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>189</v>
+        <v>244</v>
       </c>
       <c r="J74" s="2">
         <v>0</v>
       </c>
       <c r="S74" s="2" t="s">
-        <v>190</v>
+        <v>245</v>
       </c>
       <c r="T74" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.45">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20">
       <c r="A75" s="2" t="s">
-        <v>189</v>
+        <v>244</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>190</v>
+        <v>245</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>193</v>
+        <v>250</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>189</v>
+        <v>244</v>
       </c>
       <c r="J75" s="2">
         <v>888</v>
       </c>
       <c r="S75" s="2" t="s">
-        <v>190</v>
+        <v>245</v>
       </c>
       <c r="T75" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.45">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20">
       <c r="A76" s="2" t="s">
-        <v>195</v>
+        <v>252</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>196</v>
+        <v>253</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>300</v>
+        <v>254</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>195</v>
+        <v>252</v>
       </c>
       <c r="J76" s="2">
         <v>1</v>
       </c>
       <c r="S76" s="2" t="s">
-        <v>196</v>
+        <v>253</v>
       </c>
       <c r="T76" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.45">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20">
       <c r="A77" s="2" t="s">
-        <v>195</v>
+        <v>252</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>37</v>
@@ -3480,21 +3480,21 @@
         <v>0</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>196</v>
+        <v>253</v>
       </c>
       <c r="J77" s="2" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="S77" s="2" t="s">
-        <v>196</v>
+        <v>253</v>
       </c>
       <c r="T77" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.45">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20">
       <c r="A78" s="2" t="s">
-        <v>195</v>
+        <v>252</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>37</v>
@@ -3503,123 +3503,123 @@
         <v>888</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>196</v>
+        <v>253</v>
       </c>
       <c r="J78" s="2">
         <v>888</v>
       </c>
       <c r="S78" s="2" t="s">
-        <v>196</v>
+        <v>253</v>
       </c>
       <c r="T78" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.45">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20">
       <c r="A79" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="E79" s="2">
         <v>0</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J79" s="2">
         <v>777</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="M79" s="2" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="O79" s="2" t="s">
-        <v>200</v>
+        <v>259</v>
       </c>
       <c r="P79" s="2">
         <v>777</v>
       </c>
       <c r="S79" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="T79" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.45">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20">
       <c r="A80" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="E80" s="2">
         <v>888</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J80" s="2">
         <v>888</v>
       </c>
       <c r="L80" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="M80" s="2">
         <v>888</v>
       </c>
       <c r="O80" s="2" t="s">
-        <v>200</v>
+        <v>259</v>
       </c>
       <c r="P80" s="2">
         <v>888</v>
       </c>
       <c r="S80" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="T80" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.45">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20">
       <c r="A81" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="J81" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="L81" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="M81" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="S81" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T81" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="L81" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="M81" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="S81" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="T81" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.45">
+    </row>
+    <row r="82" spans="1:20">
       <c r="A82" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>37</v>
@@ -3628,21 +3628,21 @@
         <v>0</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>205</v>
+        <v>265</v>
       </c>
       <c r="J82" s="2">
         <v>777</v>
       </c>
       <c r="S82" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="T82" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.45">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20">
       <c r="A83" s="2" t="s">
-        <v>200</v>
+        <v>259</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>37</v>
@@ -3651,21 +3651,21 @@
         <v>0</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>205</v>
+        <v>265</v>
       </c>
       <c r="J83" s="2">
         <v>666</v>
       </c>
       <c r="S83" s="2" t="s">
-        <v>200</v>
+        <v>259</v>
       </c>
       <c r="T83" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.45">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20">
       <c r="A84" s="2" t="s">
-        <v>205</v>
+        <v>265</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>34</v>
@@ -3677,15 +3677,15 @@
         <v>84</v>
       </c>
       <c r="S84" s="2" t="s">
-        <v>205</v>
+        <v>265</v>
       </c>
       <c r="T84" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.45">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20">
       <c r="A85" s="2" t="s">
-        <v>205</v>
+        <v>265</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>37</v>
@@ -3694,166 +3694,166 @@
         <v>666</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>209</v>
+        <v>269</v>
       </c>
       <c r="J85" s="2">
         <v>0</v>
       </c>
       <c r="S85" s="2" t="s">
-        <v>200</v>
+        <v>259</v>
       </c>
       <c r="T85" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.45">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20">
       <c r="A86" s="2" t="s">
-        <v>211</v>
+        <v>271</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>211</v>
+        <v>271</v>
       </c>
       <c r="H86" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="J86" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="S86" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="T86" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="I86" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="J86" s="2" t="s">
+    </row>
+    <row r="87" spans="1:20">
+      <c r="A87" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="S86" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="T86" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A87" s="2" t="s">
-        <v>213</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>213</v>
+        <v>276</v>
       </c>
       <c r="H87" s="2" t="s">
         <v>277</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>212</v>
+        <v>273</v>
       </c>
       <c r="J87" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="S87" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="S87" s="2" t="s">
-        <v>213</v>
-      </c>
       <c r="T87" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.45">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20">
       <c r="A88" s="2" t="s">
-        <v>215</v>
+        <v>279</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>308</v>
+        <v>281</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>212</v>
+        <v>273</v>
       </c>
       <c r="J88" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="S88" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="T88" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20">
+      <c r="A89" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="I89" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="S88" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="T88" s="2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A89" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G89" s="2" t="s">
+      <c r="J89" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="L89" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="H89" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="I89" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="J89" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="L89" s="2" t="s">
-        <v>215</v>
-      </c>
       <c r="M89" s="2" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="S89" s="2" t="s">
-        <v>211</v>
+        <v>271</v>
       </c>
       <c r="T89" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.45">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20">
       <c r="A90" s="2" t="s">
-        <v>212</v>
+        <v>273</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="E90" s="2">
         <v>0</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>211</v>
+        <v>271</v>
       </c>
       <c r="J90" s="2" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="L90" s="2" t="s">
-        <v>213</v>
+        <v>276</v>
       </c>
       <c r="M90" s="2" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="O90" s="2" t="s">
-        <v>215</v>
+        <v>279</v>
       </c>
       <c r="P90" s="2" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="S90" s="2" t="s">
-        <v>212</v>
+        <v>273</v>
       </c>
       <c r="T90" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.45">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20">
       <c r="A91" s="2" t="s">
-        <v>217</v>
+        <v>290</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>37</v>
@@ -3862,21 +3862,21 @@
         <v>1</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>215</v>
+        <v>279</v>
       </c>
       <c r="J91" s="2">
         <v>666</v>
       </c>
       <c r="S91" s="2" t="s">
-        <v>217</v>
+        <v>290</v>
       </c>
       <c r="T91" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.45">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20">
       <c r="A92" s="2" t="s">
-        <v>215</v>
+        <v>279</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>37</v>
@@ -3885,21 +3885,21 @@
         <v>666</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>217</v>
+        <v>290</v>
       </c>
       <c r="J92" s="2">
         <v>1</v>
       </c>
       <c r="S92" s="2" t="s">
-        <v>217</v>
+        <v>290</v>
       </c>
       <c r="T92" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.45">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20">
       <c r="A93" s="2" t="s">
-        <v>220</v>
+        <v>293</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>37</v>
@@ -3908,224 +3908,224 @@
         <v>1</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>221</v>
+        <v>294</v>
       </c>
       <c r="J93" s="2">
         <v>1</v>
       </c>
       <c r="S93" s="2" t="s">
-        <v>221</v>
+        <v>294</v>
       </c>
       <c r="T93" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.45">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20">
       <c r="A94" s="2" t="s">
-        <v>220</v>
+        <v>293</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>221</v>
+        <v>294</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>223</v>
+        <v>296</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>220</v>
+        <v>293</v>
       </c>
       <c r="J94" s="2">
         <v>888</v>
       </c>
       <c r="S94" s="2" t="s">
-        <v>221</v>
+        <v>294</v>
       </c>
       <c r="T94" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.45">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20">
       <c r="A95" s="2" t="s">
-        <v>225</v>
+        <v>298</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>226</v>
+        <v>299</v>
       </c>
       <c r="E95" s="2">
         <v>2</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>227</v>
+        <v>300</v>
       </c>
       <c r="J95" s="2">
         <v>777</v>
       </c>
       <c r="L95" s="2" t="s">
-        <v>228</v>
+        <v>301</v>
       </c>
       <c r="M95" s="2">
         <v>777</v>
       </c>
       <c r="S95" s="2" t="s">
-        <v>225</v>
+        <v>298</v>
       </c>
       <c r="T95" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.45">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20">
       <c r="A96" s="2" t="s">
-        <v>225</v>
+        <v>298</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="E96" s="2">
         <v>2</v>
       </c>
       <c r="I96" s="2" t="s">
-        <v>230</v>
+        <v>303</v>
       </c>
       <c r="J96" s="2" t="s">
-        <v>236</v>
+        <v>304</v>
       </c>
       <c r="L96" s="2" t="s">
-        <v>231</v>
+        <v>305</v>
       </c>
       <c r="M96" s="2" t="s">
-        <v>236</v>
+        <v>304</v>
       </c>
       <c r="O96" s="2" t="s">
-        <v>232</v>
+        <v>306</v>
       </c>
       <c r="P96" s="2" t="s">
-        <v>236</v>
+        <v>304</v>
       </c>
       <c r="S96" s="2" t="s">
-        <v>225</v>
+        <v>298</v>
       </c>
       <c r="T96" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.45">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20">
       <c r="A97" s="2" t="s">
-        <v>230</v>
+        <v>303</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>230</v>
+        <v>303</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>339</v>
+        <v>308</v>
       </c>
       <c r="I97" s="2" t="s">
-        <v>234</v>
+        <v>309</v>
       </c>
       <c r="J97" s="2" t="s">
-        <v>235</v>
+        <v>310</v>
       </c>
       <c r="S97" s="2" t="s">
-        <v>230</v>
+        <v>303</v>
       </c>
       <c r="T97" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.45">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20">
       <c r="A98" s="2" t="s">
-        <v>231</v>
+        <v>305</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>231</v>
+        <v>305</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>337</v>
+        <v>312</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>234</v>
+        <v>309</v>
       </c>
       <c r="J98" s="2" t="s">
-        <v>290</v>
+        <v>313</v>
       </c>
       <c r="S98" s="2" t="s">
-        <v>231</v>
+        <v>305</v>
       </c>
       <c r="T98" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.45">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20">
       <c r="A99" s="2" t="s">
-        <v>232</v>
+        <v>306</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>232</v>
+        <v>306</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>338</v>
+        <v>315</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>234</v>
+        <v>309</v>
       </c>
       <c r="J99" s="2" t="s">
-        <v>291</v>
+        <v>316</v>
       </c>
       <c r="S99" s="2" t="s">
-        <v>232</v>
+        <v>306</v>
       </c>
       <c r="T99" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.45">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20">
       <c r="A100" s="2" t="s">
-        <v>234</v>
+        <v>309</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="E100" s="2">
         <v>0</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>230</v>
+        <v>303</v>
       </c>
       <c r="J100" s="2" t="s">
-        <v>296</v>
+        <v>318</v>
       </c>
       <c r="L100" s="2" t="s">
-        <v>231</v>
+        <v>305</v>
       </c>
       <c r="M100" s="2" t="s">
-        <v>296</v>
+        <v>318</v>
       </c>
       <c r="O100" s="2" t="s">
-        <v>232</v>
+        <v>306</v>
       </c>
       <c r="P100" s="2" t="s">
-        <v>296</v>
+        <v>318</v>
       </c>
       <c r="S100" s="2" t="s">
-        <v>234</v>
+        <v>309</v>
       </c>
       <c r="T100" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.45">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20">
       <c r="A101" s="2" t="s">
-        <v>238</v>
+        <v>320</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>37</v>
@@ -4134,21 +4134,21 @@
         <v>0</v>
       </c>
       <c r="I101" s="2" t="s">
-        <v>231</v>
+        <v>305</v>
       </c>
       <c r="J101" s="2" t="s">
-        <v>296</v>
+        <v>318</v>
       </c>
       <c r="S101" s="2" t="s">
-        <v>231</v>
+        <v>305</v>
       </c>
       <c r="T101" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.45">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="102" spans="1:20">
       <c r="A102" s="2" t="s">
-        <v>231</v>
+        <v>305</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>37</v>
@@ -4157,21 +4157,21 @@
         <v>777</v>
       </c>
       <c r="I102" s="2" t="s">
-        <v>238</v>
+        <v>320</v>
       </c>
       <c r="J102" s="2">
         <v>0</v>
       </c>
       <c r="S102" s="2" t="s">
-        <v>231</v>
+        <v>305</v>
       </c>
       <c r="T102" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.45">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20">
       <c r="A103" s="2" t="s">
-        <v>240</v>
+        <v>323</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>37</v>
@@ -4180,21 +4180,21 @@
         <v>0</v>
       </c>
       <c r="I103" s="2" t="s">
-        <v>232</v>
+        <v>306</v>
       </c>
       <c r="J103" s="2" t="s">
-        <v>296</v>
+        <v>318</v>
       </c>
       <c r="S103" s="2" t="s">
-        <v>232</v>
+        <v>306</v>
       </c>
       <c r="T103" s="2" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.45">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20">
       <c r="A104" s="2" t="s">
-        <v>232</v>
+        <v>306</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>37</v>
@@ -4203,160 +4203,160 @@
         <v>777</v>
       </c>
       <c r="I104" s="2" t="s">
-        <v>240</v>
+        <v>323</v>
       </c>
       <c r="J104" s="2">
         <v>0</v>
       </c>
       <c r="S104" s="2" t="s">
-        <v>232</v>
+        <v>306</v>
       </c>
       <c r="T104" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.45">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20">
       <c r="A105" s="2" t="s">
-        <v>234</v>
+        <v>309</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>234</v>
+        <v>309</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>242</v>
+        <v>326</v>
       </c>
       <c r="I105" s="2" t="s">
-        <v>238</v>
+        <v>320</v>
       </c>
       <c r="J105" s="2" t="s">
-        <v>243</v>
+        <v>327</v>
       </c>
       <c r="L105" s="2" t="s">
-        <v>240</v>
+        <v>323</v>
       </c>
       <c r="M105" s="2" t="s">
-        <v>244</v>
+        <v>328</v>
       </c>
       <c r="S105" s="2" t="s">
-        <v>234</v>
+        <v>309</v>
       </c>
       <c r="T105" s="2" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.45">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20">
       <c r="A106" s="2" t="s">
-        <v>234</v>
+        <v>309</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>238</v>
+        <v>320</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>297</v>
+        <v>330</v>
       </c>
       <c r="I106" s="2" t="s">
-        <v>234</v>
+        <v>309</v>
       </c>
       <c r="J106" s="2">
         <v>0</v>
       </c>
       <c r="S106" s="2" t="s">
-        <v>234</v>
+        <v>309</v>
       </c>
       <c r="T106" s="2" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.45">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20">
       <c r="A107" s="2" t="s">
-        <v>234</v>
+        <v>309</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>240</v>
+        <v>323</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>298</v>
+        <v>332</v>
       </c>
       <c r="I107" s="2" t="s">
-        <v>234</v>
+        <v>309</v>
       </c>
       <c r="J107" s="2">
         <v>0</v>
       </c>
       <c r="S107" s="2" t="s">
-        <v>234</v>
+        <v>309</v>
       </c>
       <c r="T107" s="2" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.45">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20">
       <c r="A108" s="2" t="s">
-        <v>248</v>
+        <v>334</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>248</v>
+        <v>334</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>249</v>
+        <v>335</v>
       </c>
       <c r="I108" s="2" t="s">
-        <v>250</v>
+        <v>336</v>
       </c>
       <c r="J108" s="2" t="s">
-        <v>251</v>
+        <v>337</v>
       </c>
       <c r="S108" s="2" t="s">
-        <v>248</v>
+        <v>334</v>
       </c>
       <c r="T108" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.45">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20">
       <c r="A109" s="2" t="s">
-        <v>250</v>
+        <v>336</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>226</v>
+        <v>299</v>
       </c>
       <c r="E109" s="2">
         <v>0</v>
       </c>
       <c r="I109" s="2" t="s">
-        <v>248</v>
+        <v>334</v>
       </c>
       <c r="J109" s="2">
         <v>777</v>
       </c>
       <c r="L109" s="2" t="s">
-        <v>253</v>
+        <v>339</v>
       </c>
       <c r="M109" s="2" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="S109" s="2" t="s">
-        <v>250</v>
+        <v>336</v>
       </c>
       <c r="T109" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.45">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20">
       <c r="A110" s="2" t="s">
-        <v>255</v>
+        <v>342</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>34</v>
@@ -4368,15 +4368,15 @@
         <v>150</v>
       </c>
       <c r="S110" s="2" t="s">
-        <v>255</v>
+        <v>342</v>
       </c>
       <c r="T110" s="2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.45">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20">
       <c r="A111" s="2" t="s">
-        <v>256</v>
+        <v>344</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>34</v>
@@ -4388,24 +4388,24 @@
         <v>100</v>
       </c>
       <c r="S111" s="2" t="s">
-        <v>256</v>
+        <v>344</v>
       </c>
       <c r="T111" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.45">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="112" spans="1:20">
       <c r="A112" s="2" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="I112" s="2" t="s">
         <v>25</v>
@@ -4414,24 +4414,24 @@
         <v>27</v>
       </c>
       <c r="S112" s="2" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="T112" s="2" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.45">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20">
       <c r="A113" s="2" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="I113" s="2" t="s">
         <v>25</v>
@@ -4440,24 +4440,24 @@
         <v>27</v>
       </c>
       <c r="S113" s="2" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="T113" s="2" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.45">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20">
       <c r="A114" s="2" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="I114" s="2" t="s">
         <v>25</v>
@@ -4466,10 +4466,10 @@
         <v>27</v>
       </c>
       <c r="S114" s="2" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="T114" s="2" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -4486,7 +4486,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4499,7 +4499,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
V1 Warning Rules update
update to QC rules for checking age at pregnancy variables - checking later ages at pregnancy are larger than earlier ages at pregnancy
</commit_message>
<xml_diff>
--- a/BCRPP_QC_R_Excel_Program/BCRPP_QC_DataDictionary_Version_1/Core QC Rules/BCRPP Warning Rules.xlsx
+++ b/BCRPP_QC_R_Excel_Program/BCRPP_QC_DataDictionary_Version_1/Core QC Rules/BCRPP Warning Rules.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28208"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{FF3ECAE6-FA59-42D9-A401-5BC2971A3674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C71F37B-A02F-4CC5-9366-8D3BE64C24FD}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{FF3ECAE6-FA59-42D9-A401-5BC2971A3674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D30B4A8B-4DE2-46C9-9CD8-FF2734DD4628}"/>
   <bookViews>
     <workbookView xWindow="-76920" yWindow="-5820" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -359,7 +359,7 @@
     <t>parity == 2 &amp; parity != 888 &amp; parity != 777</t>
   </si>
   <si>
-    <t>parity is 2, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
+    <t>parity is 2, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy (e.g, age_preg2 &gt; age_preg1)</t>
   </si>
   <si>
     <t>age_preg3,age_preg2,age_preg1</t>
@@ -371,73 +371,73 @@
     <t>parity ==3 &amp; parity != 888 &amp; parity != 777</t>
   </si>
   <si>
-    <t>parity is 3, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
+    <t>parity is 3, please check if 666 was accidentally entered as a value for age at pregancy; or if later ages at pregnancy should be greater than the earlier ages at pregnancy (e.g, age_preg3 &gt; age_preg2)</t>
   </si>
   <si>
     <t>age_preg4,age_preg3,age_preg2,age_preg1</t>
   </si>
   <si>
-    <t>!age_preg4 %in% c(666) &amp; age_preg4 &gt; age_preg3 &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666)   | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 | age_preg1 == 888</t>
+    <t>!age_preg4 %in% c(666) &amp; age_preg4 &gt; age_preg3 &amp; age_preg3 &gt; age_preg2 &amp; age_preg2 &gt; age_preg1 &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666)   | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 | age_preg1 == 888</t>
   </si>
   <si>
     <t>parity ==4 &amp; parity != 888 &amp; parity != 777</t>
   </si>
   <si>
-    <t>parity is 4, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
+    <t>parity is 4, please check if 666 was accidentally entered as a value for age at pregancy; or if later ages at pregnancy should be greater than the earlier ages at pregnancy (e.g, age_preg3 &gt; age_preg2)</t>
   </si>
   <si>
     <t>age_preg5,age_preg4,age_preg3,age_preg2,age_preg1</t>
   </si>
   <si>
-    <t>!age_preg5 %in% c(666) &amp; age_preg5 &gt; age_preg4 &amp; !age_preg4 %in% c(666) &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666)  | age_preg5 == 888| age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 | age_preg1 == 888</t>
+    <t>!age_preg5 %in% c(666) &amp; age_preg5 &gt; age_preg4 &amp; age_preg4 &gt; age_preg3 &amp; age_preg3 &gt; age_preg2 &amp; age_preg2 &gt; age_preg1 &amp; !age_preg4 %in% c(666) &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666)  | age_preg5 == 888| age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 | age_preg1 == 888</t>
   </si>
   <si>
     <t>parity ==5 &amp; parity != 888 &amp; parity != 777</t>
   </si>
   <si>
-    <t>parity is 5, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
+    <t>parity is 5, please check if 666 was accidentally entered as a value for age at pregancy; or if later ages at pregnancy should be greater than the earlier ages at pregnancy (e.g, age_preg3 &gt; age_preg2)</t>
   </si>
   <si>
     <t>age_preg6,age_preg5,age_preg4,age_preg3,age_preg2,age_preg1</t>
   </si>
   <si>
-    <t>!age_preg6 %in% c(666) &amp; age_preg6 &gt; age_preg5 &amp; !age_preg5 %in% c(666) &amp; !age_preg4 %in% c(666) &amp; !age_preg3 %in% c(666)&amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666) | age_preg6 == 888 | age_preg5 == 888 | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 | age_preg1 == 888</t>
+    <t>!age_preg6 %in% c(666) &amp; age_preg6 &gt; age_preg5 &amp; age_preg5 &gt; age_preg4 &amp; age_preg4 &gt; age_preg3 &amp; age_preg3 &gt; age_preg2 &amp; age_preg2 &gt; age_preg1 &amp; !age_preg5 %in% c(666) &amp; !age_preg4 %in% c(666) &amp; !age_preg3 %in% c(666)&amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666) | age_preg6 == 888 | age_preg5 == 888 | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 | age_preg1 == 888</t>
   </si>
   <si>
     <t>parity ==6 &amp; parity != 888 &amp; parity != 777</t>
   </si>
   <si>
-    <t>parity is 6, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
+    <t>parity is 6, please check if 666 was accidentally entered as a value for age at pregancy; or if later ages at pregnancy should be greater than the earlier ages at pregnancy (e.g, age_preg3 &gt; age_preg2)</t>
   </si>
   <si>
     <t>age_preg7,age_preg6,age_preg5,age_preg4,age_preg3,age_preg2,age_preg1</t>
   </si>
   <si>
-    <t>!age_preg7 %in% c(666) &amp; age_preg7 &gt; age_preg6 &amp; !age_preg6 %in% c(666)  &amp; !age_preg5 %in% c(666) &amp; !age_preg4  %in% c(666)  &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666) | age_preg7 == 888 | age_preg6 == 888 | age_preg5 == 888 | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 |age_preg1 == 888</t>
+    <t>!age_preg7 %in% c(666) &amp; age_preg7 &gt; age_preg6 &amp; age_preg6 &gt; age_preg5 &amp; age_preg5 &gt; age_preg4 &amp; age_preg4 &gt; age_preg3 &amp; age_preg3 &gt; age_preg2 &amp; age_preg2 &gt; age_preg1 &amp; !age_preg6 %in% c(666)  &amp; !age_preg5 %in% c(666) &amp; !age_preg4  %in% c(666)  &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666) | age_preg7 == 888 | age_preg6 == 888 | age_preg5 == 888 | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 |age_preg1 == 888</t>
   </si>
   <si>
     <t>parity ==7 &amp; parity != 888 &amp; parity != 777</t>
   </si>
   <si>
-    <t>parity is 7, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
+    <t>parity is 7, please check if 666 was accidentally entered as a value for age at pregancy; or if later ages at pregnancy should be greater than the earlier ages at pregnancy (e.g, age_preg3 &gt; age_preg2)</t>
   </si>
   <si>
     <t>age_preg8,age_preg7,age_preg6,age_preg5,age_preg4,age_preg3,age_preg2,age_preg1</t>
   </si>
   <si>
-    <t>!age_preg8 %in% c(666) &amp; age_preg8 &gt; age_preg7 &amp; !age_preg7 %in% c(666)  &amp; !age_preg6 %in% c(666) &amp; !age_preg5 %in% c(666)  &amp; !age_preg4 %in% c(666)  &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666)  | age_preg8 == 888 | age_preg7 == 888 | age_preg6 == 888 | age_preg5 == 888 | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 |age_preg1 == 888</t>
+    <t>!age_preg8 %in% c(666) &amp; age_preg8 &gt; age_preg7 &amp; age_preg7 &gt; age_preg6 &amp; age_preg6 &gt; age_preg5 &amp; age_preg5 &gt; age_preg4 &amp; age_preg4 &gt; age_preg3 &amp; age_preg3 &gt; age_preg2 &amp; age_preg2 &gt; age_preg1 &amp; !age_preg7 %in% c(666)  &amp; !age_preg6 %in% c(666) &amp; !age_preg5 %in% c(666)  &amp; !age_preg4 %in% c(666)  &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666)  | age_preg8 == 888 | age_preg7 == 888 | age_preg6 == 888 | age_preg5 == 888 | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 |age_preg1 == 888</t>
   </si>
   <si>
     <t>parity ==8 &amp; parity != 888 &amp; parity != 777</t>
   </si>
   <si>
-    <t>parity is 8, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
+    <t>parity is 8, please check if 666 was accidentally entered as a value for age at pregancy; or if later ages at pregnancy should be greater than the earlier ages at pregnancy (e.g, age_preg3 &gt; age_preg2)</t>
   </si>
   <si>
     <t>age_preg9,age_preg8,age_preg7,age_preg6,age_preg5,age_preg4,age_preg3,age_preg2,age_preg1</t>
   </si>
   <si>
-    <t>!age_preg9 %in% c(666) &amp; age_preg9 &gt; age_preg8 &amp; !age_preg8 %in% c(666) &amp; !age_preg7 %in% c(666)  &amp; !age_preg6 %in% c(666) &amp; !age_preg5 %in% c(666) &amp; !age_preg4 %in% c(666) &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666) | age_preg9 == 888 | age_preg8 == 888 | age_preg7 == 888 | age_preg6 == 888 | age_preg5 == 888 | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 | age_preg1 == 888</t>
+    <t>!age_preg9 %in% c(666) &amp; age_preg9 &gt; age_preg8 &amp; age_preg8 &gt; age_preg7 &amp; age_preg7 &gt; age_preg6 &amp; age_preg6 &gt; age_preg5 &amp; age_preg5 &gt; age_preg4 &amp; age_preg4 &gt; age_preg3 &amp; age_preg3 &gt; age_preg2 &amp; age_preg2 &gt; age_preg1 &amp; !age_preg8 %in% c(666) &amp; !age_preg7 %in% c(666)  &amp; !age_preg6 %in% c(666) &amp; !age_preg5 %in% c(666) &amp; !age_preg4 %in% c(666) &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666) | age_preg9 == 888 | age_preg8 == 888 | age_preg7 == 888 | age_preg6 == 888 | age_preg5 == 888 | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 | age_preg1 == 888</t>
   </si>
   <si>
     <t xml:space="preserve">parity </t>
@@ -446,19 +446,19 @@
     <t>parity ==9 &amp; parity != 888 &amp; parity != 777</t>
   </si>
   <si>
-    <t>parity is 9, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
+    <t>parity is 9, please check if 666 was accidentally entered as a value for age at pregancy; or if later ages at pregnancy should be greater than the earlier ages at pregnancy (e.g, age_preg3 &gt; age_preg2)</t>
   </si>
   <si>
     <t>age_preg10,age_preg9,age_preg8,age_preg7,age_preg6,age_preg5,age_preg4,age_preg3,age_preg2,age_preg1</t>
   </si>
   <si>
-    <t>!age_preg10 %in% c(666) &amp; age_preg10 &gt; age_preg9 &amp; !age_preg9 %in% c(666) &amp; !age_preg8 %in% c(666) &amp; !age_preg7 %in% c(666) &amp;  !age_preg6 %in% c(666)  &amp; !age_preg5 %in% c(666)  &amp; !age_preg4 %in% c(666) &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666)  | age_preg10 == 888 | age_preg9 == 888 | age_preg8 == 888 | age_preg7 == 888 | age_preg7 == 888 | age_preg6 == 888 | age_preg5 == 888 | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 | age_preg1 == 888</t>
+    <t>!age_preg10 %in% c(666) &amp; age_preg10 &gt; age_preg9 &amp; age_preg9 &gt; age_preg8 &amp; age_preg8 &gt; age_preg7 &amp; age_preg7 &gt; age_preg6 &amp; age_preg6 &gt; age_preg5 &amp; age_preg5 &gt; age_preg4 &amp; age_preg4 &gt; age_preg3 &amp; age_preg3 &gt; age_preg2 &amp; age_preg2 &gt; age_preg1 &amp;  !age_preg9 %in% c(666) &amp; !age_preg8 %in% c(666) &amp; !age_preg7 %in% c(666) &amp;  !age_preg6 %in% c(666)  &amp; !age_preg5 %in% c(666)  &amp; !age_preg4 %in% c(666) &amp; !age_preg3 %in% c(666) &amp; !age_preg2 %in% c(666) &amp; !age_preg1 %in% c(666)  | age_preg10 == 888 | age_preg9 == 888 | age_preg8 == 888 | age_preg7 == 888 | age_preg7 == 888 | age_preg6 == 888 | age_preg5 == 888 | age_preg4 == 888 | age_preg3 == 888 | age_preg2 == 888 | age_preg1 == 888</t>
   </si>
   <si>
     <t>parity &gt;=10 &amp; parity != 888 &amp; parity != 777</t>
   </si>
   <si>
-    <t>parity is 10, please check if 666 was accidentally entered as a value for age at pregancy; or if later age at pregnancy should be greater than the previous age at pregnancy.</t>
+    <t>parity is 10, please check if 666 was accidentally entered as a value for age at pregancy; or if later ages at pregnancy should be greater than the earlier ages at pregnancy (e.g, age_preg3 &gt; age_preg2)</t>
   </si>
   <si>
     <t>breastfeed_dur_b1</t>
@@ -740,7 +740,7 @@
     <t xml:space="preserve"> !smoking_stop %in% c(666,777,888)</t>
   </si>
   <si>
-    <t>smoking_dur is more than the difference between smoking_init and smoking_stop ± 4 year window</t>
+    <t>smoking_dur is more than the difference between smoking_init and smoking_stop ± 2 year window</t>
   </si>
   <si>
     <t xml:space="preserve">smoking_init </t>
@@ -1470,34 +1470,34 @@
   <dimension ref="A1:U114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B56" sqref="B56"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="T31" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="T36" sqref="T36"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.600000000000001"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="119.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="255.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="45.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="64.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="180" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="128.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="365.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="49" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="69" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="35.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="25.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="192.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>

</xml_diff>